<commit_message>
Modificaciones en la plantilla de reportes
</commit_message>
<xml_diff>
--- a/PortalRoemmers/Import/SolicitudRRHH/PlantillaVacacionesPortal2023.xlsx
+++ b/PortalRoemmers/Import/SolicitudRRHH/PlantillaVacacionesPortal2023.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljara1\source\repos\PortalRoemmers\PortalRoemmers\Import\SolicitudRRHH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81C99A8-4133-423C-A232-B1DA9A7D1FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7BB91E-632A-4B7D-AC0C-40BE890C864C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="2340" windowWidth="21465" windowHeight="8190" xr2:uid="{270724AE-1FAE-4D31-B8F0-99EEC24A0EA9}"/>
+    <workbookView xWindow="1320" yWindow="705" windowWidth="21465" windowHeight="11835" xr2:uid="{270724AE-1FAE-4D31-B8F0-99EEC24A0EA9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -468,7 +468,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>